<commit_message>
actualizacion de informaicon relevante
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/transaction_data.xlsx
+++ b/src/test/resources/testdata/transaction_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rootstack\POC\Automatizacion\POC\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743A0C0-4442-4DBA-8ABB-A427FEC8B0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85843441-9F91-4BCB-8DB4-116322C5BC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{75286747-2714-40F6-B5B3-353E88CBCB6D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75286747-2714-40F6-B5B3-353E88CBCB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,10 +518,10 @@
         <v>98</v>
       </c>
       <c r="E2">
-        <v>1.2612000000000001</v>
+        <v>1.2624</v>
       </c>
       <c r="F2">
-        <v>126.12</v>
+        <v>126.24</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -536,7 +536,7 @@
         <v>15</v>
       </c>
       <c r="K2">
-        <v>1234565789</v>
+        <v>1234956578</v>
       </c>
       <c r="L2" t="s">
         <v>16</v>

</xml_diff>